<commit_message>
Leveling_base + crit chance 1% => 10%
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Witch Killer's Blade</t>
+  </si>
+  <si>
+    <t>nothing</t>
   </si>
 </sst>
 </file>
@@ -689,10 +692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,98 +718,98 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1.1499999999999999</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>1.03</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>1.07</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1.1000000000000001</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>1.1499999999999999</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9">
-        <v>1.25</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>1.25</v>
@@ -814,23 +817,34 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
       <c r="C11">
-        <v>1.35</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>7</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>1.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Map_base + armor_base + some additions in lists-script and mode_select
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\PycharmProjects\RPG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\008\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
     <sheet name="guns" sheetId="2" r:id="rId2"/>
+    <sheet name="locations" sheetId="3" r:id="rId3"/>
+    <sheet name="armor" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -121,6 +123,84 @@
   </si>
   <si>
     <t>nothing</t>
+  </si>
+  <si>
+    <t>lvl</t>
+  </si>
+  <si>
+    <t>monsterlvl</t>
+  </si>
+  <si>
+    <t>Starting Village</t>
+  </si>
+  <si>
+    <t>The Road</t>
+  </si>
+  <si>
+    <t>Dark Cave</t>
+  </si>
+  <si>
+    <t>Evil Woods</t>
+  </si>
+  <si>
+    <t>Yormungard</t>
+  </si>
+  <si>
+    <t>Desert of Time</t>
+  </si>
+  <si>
+    <t>Bandit Camp</t>
+  </si>
+  <si>
+    <t>The Canyon</t>
+  </si>
+  <si>
+    <t>The Abyss</t>
+  </si>
+  <si>
+    <t>Vampire Castle</t>
+  </si>
+  <si>
+    <t>dodge</t>
+  </si>
+  <si>
+    <t>Leather Armor</t>
+  </si>
+  <si>
+    <t>Iron Armor</t>
+  </si>
+  <si>
+    <t>Rags</t>
+  </si>
+  <si>
+    <t>Armored Clothes</t>
+  </si>
+  <si>
+    <t>Chainmail</t>
+  </si>
+  <si>
+    <t>Copper Armor</t>
+  </si>
+  <si>
+    <t>golddrop</t>
+  </si>
+  <si>
+    <t>Steel Armor</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Assassin's Armor</t>
+  </si>
+  <si>
+    <t>Pirate's Hat</t>
+  </si>
+  <si>
+    <t>Igi's Armor</t>
+  </si>
+  <si>
+    <t>equipment</t>
   </si>
 </sst>
 </file>
@@ -447,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +541,7 @@
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,13 +554,19 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -488,13 +574,19 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -502,13 +594,19 @@
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -516,13 +614,19 @@
       <c r="D4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -530,13 +634,19 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -544,13 +654,19 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -558,13 +674,19 @@
       <c r="D7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -572,13 +694,19 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -586,13 +714,19 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -600,13 +734,19 @@
       <c r="D10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -614,27 +754,39 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
         <v>7</v>
       </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -642,13 +794,19 @@
       <c r="D13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -656,13 +814,19 @@
       <c r="D14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>7</v>
@@ -670,19 +834,31 @@
       <c r="D15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>10</v>
       </c>
       <c r="D16">
         <v>7</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -692,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +881,7 @@
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -715,8 +891,11 @@
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -726,8 +905,11 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -737,8 +919,11 @@
       <c r="C3">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -748,8 +933,11 @@
       <c r="C4">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -759,8 +947,11 @@
       <c r="C5">
         <v>1.03</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -770,8 +961,11 @@
       <c r="C6">
         <v>1.07</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -781,8 +975,11 @@
       <c r="C7">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -792,8 +989,11 @@
       <c r="C8">
         <v>1.05</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -803,8 +1003,11 @@
       <c r="C9">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -814,8 +1017,11 @@
       <c r="C10">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -825,8 +1031,11 @@
       <c r="C11">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -836,8 +1045,11 @@
       <c r="C12">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -846,6 +1058,322 @@
       </c>
       <c r="C13">
         <v>1.25</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.95</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0.9</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0.7</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.6</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1.6</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Market not working. Debug needed.
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
     <sheet name="guns" sheetId="2" r:id="rId2"/>
     <sheet name="locations" sheetId="3" r:id="rId3"/>
     <sheet name="armor" sheetId="4" r:id="rId4"/>
+    <sheet name="loot" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>name</t>
   </si>
@@ -201,6 +202,48 @@
   </si>
   <si>
     <t>Nightingale's dagger</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>stone</t>
+  </si>
+  <si>
+    <t>iron ore</t>
+  </si>
+  <si>
+    <t>wooden stick</t>
+  </si>
+  <si>
+    <t>rusty dagger</t>
+  </si>
+  <si>
+    <t>monster egg</t>
+  </si>
+  <si>
+    <t>feather</t>
+  </si>
+  <si>
+    <t>coin</t>
+  </si>
+  <si>
+    <t>gold nugget</t>
+  </si>
+  <si>
+    <t>metal scrap</t>
+  </si>
+  <si>
+    <t>soul gem</t>
+  </si>
+  <si>
+    <t>katana</t>
+  </si>
+  <si>
+    <t>map to abyss</t>
+  </si>
+  <si>
+    <t>magic essence</t>
   </si>
 </sst>
 </file>
@@ -868,10 +911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +924,7 @@
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -894,8 +937,11 @@
       <c r="D1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -906,38 +952,47 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1.05</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1.1499999999999999</v>
+        <v>1.35</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -945,13 +1000,16 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>1.03</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -959,13 +1017,16 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1.07</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -973,13 +1034,16 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -992,8 +1056,11 @@
       <c r="D8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1001,13 +1068,16 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <v>1.1499999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="D9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -1015,13 +1085,16 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>1.25</v>
+        <v>1.35</v>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1029,13 +1102,16 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="D11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1043,13 +1119,16 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>1.35</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1057,10 +1136,13 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <v>1.25</v>
+        <v>1.3</v>
       </c>
       <c r="D13">
         <v>10</v>
+      </c>
+      <c r="E13">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -1181,7 +1263,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1261,7 +1343,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1270,18 +1352,18 @@
         <v>0.95</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>0.9</v>
@@ -1290,7 +1372,7 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1349,7 +1431,7 @@
         <v>43</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>1.5</v>
@@ -1366,10 +1448,10 @@
         <v>44</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -1392,7 +1474,179 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <v>350</v>
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost everything works. Need to update save-load system and some player interactions
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>name</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>lvl</t>
-  </si>
-  <si>
-    <t>monsterlvl</t>
   </si>
   <si>
     <t>Starting Village</t>
@@ -572,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -661,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -938,12 +935,12 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -960,7 +957,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -977,7 +974,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -994,7 +991,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1011,7 +1008,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1028,7 +1025,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1045,7 +1042,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -1062,7 +1059,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -1079,7 +1076,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1096,7 +1093,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -1113,7 +1110,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -1155,7 +1152,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,12 +1167,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1183,7 +1180,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1191,7 +1188,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1199,7 +1196,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1207,7 +1204,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1215,7 +1212,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1223,7 +1220,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1231,7 +1228,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1239,7 +1236,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1247,7 +1244,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1275,24 +1272,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1309,7 +1306,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1326,7 +1323,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1343,7 +1340,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1360,7 +1357,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -1377,7 +1374,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1394,7 +1391,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -1411,7 +1408,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -1428,7 +1425,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1445,7 +1442,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1462,7 +1459,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1486,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1500,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
@@ -1508,7 +1505,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1519,7 +1516,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1530,7 +1527,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1541,7 +1538,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1552,7 +1549,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1563,7 +1560,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1574,7 +1571,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1585,7 +1582,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -1596,7 +1593,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -1607,7 +1604,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1618,7 +1615,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>15</v>
@@ -1629,7 +1626,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -1640,7 +1637,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14">
         <v>100</v>

</xml_diff>

<commit_message>
Made something, idk. Maybe... alpha?
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
   <si>
     <t>name</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>magic essence</t>
+  </si>
+  <si>
+    <t>№</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -908,10 +911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +924,7 @@
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -937,8 +940,11 @@
       <c r="E1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -954,8 +960,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -971,8 +980,11 @@
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -988,8 +1000,11 @@
       <c r="E4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1005,8 +1020,11 @@
       <c r="E5">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1022,8 +1040,11 @@
       <c r="E6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -1039,8 +1060,11 @@
       <c r="E7">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1056,8 +1080,11 @@
       <c r="E8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1073,8 +1100,11 @@
       <c r="E9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -1090,8 +1120,11 @@
       <c r="E10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1107,8 +1140,11 @@
       <c r="E11">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1124,8 +1160,11 @@
       <c r="E12">
         <v>300</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1140,6 +1179,9 @@
       </c>
       <c r="E13">
         <v>500</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1257,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1312,7 @@
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1286,8 +1328,11 @@
       <c r="E1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1303,8 +1348,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1320,8 +1368,11 @@
       <c r="E3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1337,8 +1388,11 @@
       <c r="E4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1354,8 +1408,11 @@
       <c r="E5">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1371,8 +1428,11 @@
       <c r="E6">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1388,8 +1448,11 @@
       <c r="E7">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1405,8 +1468,11 @@
       <c r="E8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1422,8 +1488,11 @@
       <c r="E9">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1439,8 +1508,11 @@
       <c r="E10">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1456,8 +1528,11 @@
       <c r="E11">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1472,6 +1547,9 @@
       </c>
       <c r="E12">
         <v>1000</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored attack and vivod func. A few bugfixes.
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7440" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="enemies" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>name</t>
   </si>
@@ -913,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1559,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1570,7 @@
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1580,8 +1580,11 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1591,8 +1594,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1602,8 +1608,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1613,8 +1622,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1624,8 +1636,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1635,8 +1650,11 @@
       <c r="C6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1646,8 +1664,11 @@
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1657,8 +1678,11 @@
       <c r="C8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1668,8 +1692,11 @@
       <c r="C9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1679,8 +1706,11 @@
       <c r="C10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1690,8 +1720,11 @@
       <c r="C11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1701,8 +1734,11 @@
       <c r="C12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1712,8 +1748,11 @@
       <c r="C13">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -1722,6 +1761,9 @@
       </c>
       <c r="C14">
         <v>8</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>